<commit_message>
Finished adding the 18 data points
</commit_message>
<xml_diff>
--- a/PerformanceExcelSheet.xlsx
+++ b/PerformanceExcelSheet.xlsx
@@ -407,7 +407,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,78 +1069,203 @@
       <c r="G16" s="2">
         <v>9635</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="H16" s="2">
+        <v>26228</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.26866099999999998</v>
+      </c>
+      <c r="J16" s="2">
+        <v>127027</v>
+      </c>
       <c r="K16" s="2">
         <v>34752</v>
       </c>
       <c r="L16" s="2">
         <v>7044</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="M16" s="2">
+        <v>1490</v>
+      </c>
+      <c r="N16" s="4">
+        <v>3.655243</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
       <c r="F17" s="2">
         <v>35863</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="G17" s="2">
+        <v>30303</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5560</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.84496599999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>314529</v>
+      </c>
       <c r="K17" s="2">
         <v>34752</v>
       </c>
       <c r="L17" s="2">
         <v>7044</v>
       </c>
-      <c r="N17" s="4"/>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>9.0506729999999997</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
       <c r="F18" s="2">
         <v>35863</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="G18" s="2">
+        <v>30303</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5560</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.84496599999999999</v>
+      </c>
+      <c r="J18" s="2">
+        <v>307485</v>
+      </c>
       <c r="K18" s="2">
         <v>34752</v>
       </c>
       <c r="L18" s="2">
         <v>7044</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="M18" s="2">
+        <v>7044</v>
+      </c>
+      <c r="N18" s="4">
+        <v>8.8479799999999997</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
       <c r="F19" s="2">
         <v>35863</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="G19" s="2">
+        <v>35766</v>
+      </c>
+      <c r="H19" s="2">
+        <v>97</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0.99729500000000004</v>
+      </c>
+      <c r="J19" s="2">
+        <v>363696</v>
+      </c>
       <c r="K19" s="2">
         <v>34752</v>
       </c>
       <c r="L19" s="2">
         <v>7044</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>10.46547</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
       <c r="F20" s="2">
         <v>35863</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="G20" s="2">
+        <v>35766</v>
+      </c>
+      <c r="H20" s="2">
+        <v>97</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.99729500000000004</v>
+      </c>
+      <c r="J20" s="2">
+        <v>356652</v>
+      </c>
       <c r="K20" s="2">
         <v>34752</v>
       </c>
       <c r="L20" s="2">
         <v>7044</v>
       </c>
-      <c r="N20" s="4"/>
+      <c r="M20" s="2">
+        <v>7044</v>
+      </c>
+      <c r="N20" s="4">
+        <v>10.262776000000001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated TAKEN pipeline numbers
</commit_message>
<xml_diff>
--- a/PerformanceExcelSheet.xlsx
+++ b/PerformanceExcelSheet.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Microsoft\Documents\GitHub\CompOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinhak\Documents\GitHub\CompOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9885" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9888" windowHeight="9492"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -675,31 +675,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,6 +707,246 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dashDot">
+          <color indexed="64"/>
+        </left>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="dashDot">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="dashDotDot">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dashDotDot">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -727,253 +967,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dashDot">
-          <color indexed="64"/>
-        </left>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="dashDot">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="dashDotDot">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dashDotDot">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <right style="thick">
           <color indexed="64"/>
@@ -988,6 +981,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1016,26 +1016,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:N33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:N33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="A2:N33"/>
   <sortState ref="A3:N33">
     <sortCondition ref="A2:A33"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Test #" dataDxfId="0"/>
-    <tableColumn id="2" name="Cache Size (index)" dataDxfId="13"/>
-    <tableColumn id="3" name="Blocksize" dataDxfId="12"/>
-    <tableColumn id="4" name="Level of Association" dataDxfId="11"/>
-    <tableColumn id="5" name="Taken/Not-taken" dataDxfId="10"/>
-    <tableColumn id="6" name="Num of Cache Accesses" dataDxfId="9"/>
-    <tableColumn id="7" name="Num of Cache Misses" dataDxfId="8"/>
-    <tableColumn id="8" name="Num of Cache Hits" dataDxfId="7"/>
-    <tableColumn id="9" name="Cache Miss Rate" dataDxfId="6"/>
-    <tableColumn id="10" name="Total Cycles" dataDxfId="5"/>
-    <tableColumn id="11" name="Total Instructions" dataDxfId="4"/>
-    <tableColumn id="12" name="Total Branch Instructions" dataDxfId="3"/>
-    <tableColumn id="13" name="Total Correct Branch Predictions" dataDxfId="2"/>
-    <tableColumn id="14" name="CPI" dataDxfId="1"/>
+    <tableColumn id="1" name="Test #" dataDxfId="13"/>
+    <tableColumn id="2" name="Cache Size (index)" dataDxfId="12"/>
+    <tableColumn id="3" name="Blocksize" dataDxfId="11"/>
+    <tableColumn id="4" name="Level of Association" dataDxfId="10"/>
+    <tableColumn id="5" name="Taken/Not-taken" dataDxfId="9"/>
+    <tableColumn id="6" name="Num of Cache Accesses" dataDxfId="8"/>
+    <tableColumn id="7" name="Num of Cache Misses" dataDxfId="7"/>
+    <tableColumn id="8" name="Num of Cache Hits" dataDxfId="6"/>
+    <tableColumn id="9" name="Cache Miss Rate" dataDxfId="5"/>
+    <tableColumn id="10" name="Total Cycles" dataDxfId="4"/>
+    <tableColumn id="11" name="Total Instructions" dataDxfId="3"/>
+    <tableColumn id="12" name="Total Branch Instructions" dataDxfId="2"/>
+    <tableColumn id="13" name="Total Correct Branch Predictions" dataDxfId="1"/>
+    <tableColumn id="14" name="CPI" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1310,51 +1310,51 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="11.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="18.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.109375" style="1"/>
+    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="33" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="32" t="s">
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="35"/>
-    </row>
-    <row r="2" spans="1:14" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="40"/>
+    </row>
+    <row r="2" spans="1:14" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1438,11 +1438,11 @@
       <c r="M3" s="5">
         <v>0</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="32">
         <v>10.490589999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>2</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="7">
-        <v>357525</v>
+        <v>364569</v>
       </c>
       <c r="K4" s="4">
         <v>34752</v>
@@ -1483,10 +1483,10 @@
         <v>7044</v>
       </c>
       <c r="N4" s="17">
-        <v>10.287896999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.490589999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>5.5295230000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>0.47932399999999997</v>
       </c>
       <c r="J6" s="7">
-        <v>193818</v>
+        <v>196512</v>
       </c>
       <c r="K6" s="4">
         <v>34752</v>
@@ -1568,13 +1568,13 @@
         <v>7044</v>
       </c>
       <c r="M6" s="4">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18">
-        <v>5.5771750000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.6546960000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>7.3750580000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>0.68176099999999995</v>
       </c>
       <c r="J8" s="7">
-        <v>260362</v>
+        <v>261852</v>
       </c>
       <c r="K8" s="4">
         <v>34752</v>
@@ -1656,13 +1656,13 @@
         <v>7044</v>
       </c>
       <c r="M8" s="4">
-        <v>1490</v>
+        <v>0</v>
       </c>
       <c r="N8" s="18">
-        <v>7.492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7.5348759999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>2.1066410000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>0.11359900000000001</v>
       </c>
       <c r="J10" s="7">
-        <v>76882</v>
+        <v>77291</v>
       </c>
       <c r="K10" s="4">
         <v>34752</v>
@@ -1744,13 +1744,13 @@
         <v>7044</v>
       </c>
       <c r="M10" s="4">
-        <v>1686</v>
+        <v>1277</v>
       </c>
       <c r="N10" s="18">
-        <v>2.212304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.2240730000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>5.5295230000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>0.47932399999999997</v>
       </c>
       <c r="J12" s="7">
-        <v>193818</v>
+        <v>196512</v>
       </c>
       <c r="K12" s="4">
         <v>34752</v>
@@ -1832,13 +1832,13 @@
         <v>7044</v>
       </c>
       <c r="M12" s="4">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="N12" s="18">
-        <v>5.5771499999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.6546960000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>2.1066410000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>0.11359900000000001</v>
       </c>
       <c r="J14" s="7">
-        <v>76882</v>
+        <v>77291</v>
       </c>
       <c r="K14" s="4">
         <v>34752</v>
@@ -1920,13 +1920,13 @@
         <v>7044</v>
       </c>
       <c r="M14" s="4">
-        <v>1686</v>
+        <v>1277</v>
       </c>
       <c r="N14" s="18">
-        <v>2.212304</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.2240730000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>3.5383</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>0.26866099999999998</v>
       </c>
       <c r="J16" s="7">
-        <v>127027</v>
+        <v>127267</v>
       </c>
       <c r="K16" s="4">
         <v>34752</v>
@@ -2008,13 +2008,13 @@
         <v>7044</v>
       </c>
       <c r="M16" s="4">
-        <v>1490</v>
+        <v>1250</v>
       </c>
       <c r="N16" s="18">
-        <v>3.655243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.6621489999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>9.0506729999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0.84496599999999999</v>
       </c>
       <c r="J18" s="7">
-        <v>307485</v>
+        <v>314529</v>
       </c>
       <c r="K18" s="4">
         <v>34752</v>
@@ -2096,13 +2096,13 @@
         <v>7044</v>
       </c>
       <c r="M18" s="4">
-        <v>7044</v>
+        <v>0</v>
       </c>
       <c r="N18" s="18">
-        <v>8.8479799999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>9.0506729999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>10.46547</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0.99729500000000004</v>
       </c>
       <c r="J20" s="7">
-        <v>356652</v>
+        <v>363696</v>
       </c>
       <c r="K20" s="4">
         <v>34752</v>
@@ -2184,13 +2184,13 @@
         <v>7044</v>
       </c>
       <c r="M20" s="4">
-        <v>7044</v>
+        <v>0</v>
       </c>
       <c r="N20" s="18">
-        <v>10.262776000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.46547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>1.577377</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>3.0728589999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>1.3154349999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>1.3154349999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>1.3154349999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>2.9418E-2</v>
       </c>
       <c r="J26" s="7">
-        <v>50092</v>
+        <v>50133</v>
       </c>
       <c r="K26" s="4">
         <v>34752</v>
@@ -2448,14 +2448,14 @@
         <v>7044</v>
       </c>
       <c r="M26" s="4">
-        <v>1333</v>
+        <v>1292</v>
       </c>
       <c r="N26" s="17">
-        <v>1.4414130000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="40">
+        <v>1.442593</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="36">
         <v>25</v>
       </c>
       <c r="B27" s="12">
@@ -2498,7 +2498,7 @@
         <v>1.577377</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>26</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>1.242375</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>27</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>1.2440150000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>28</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>1.401473</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>29</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>10.490589999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>30</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>2.1163999999999999E-2</v>
       </c>
       <c r="J32" s="7">
-        <v>47553</v>
+        <v>47594</v>
       </c>
       <c r="K32" s="4">
         <v>34752</v>
@@ -2712,13 +2712,13 @@
         <v>7044</v>
       </c>
       <c r="M32" s="4">
-        <v>1333</v>
+        <v>1292</v>
       </c>
       <c r="N32" s="18">
-        <v>1.3683529999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.3695329999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>1.3738779999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F34"/>
       <c r="I34" s="3"/>
       <c r="K34"/>
@@ -2770,7 +2770,7 @@
       <c r="M34"/>
       <c r="N34"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F35"/>
       <c r="I35" s="3"/>
       <c r="K35"/>
@@ -2778,21 +2778,21 @@
       <c r="M35"/>
       <c r="N35"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G42"/>
       <c r="H42"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G43"/>
       <c r="H43"/>
     </row>

</xml_diff>